<commit_message>
Klickabfolge - Szene 7 quiz updated
</commit_message>
<xml_diff>
--- a/Klickabfolge Tabelle Szene 1-7.xlsx
+++ b/Klickabfolge Tabelle Szene 1-7.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1263" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1315" uniqueCount="222">
   <si>
     <t>Interact</t>
   </si>
@@ -578,13 +578,157 @@
   </si>
   <si>
     <t>Quiz gelöst</t>
+  </si>
+  <si>
+    <t>QUIZ:</t>
+  </si>
+  <si>
+    <t>FRAGE1:</t>
+  </si>
+  <si>
+    <t>FRAGE2:</t>
+  </si>
+  <si>
+    <t>FRAGE3:</t>
+  </si>
+  <si>
+    <t>FRAGE4</t>
+  </si>
+  <si>
+    <t>Wie sollten in sozialen Netzwerken meine Privatsphäre-Einstellungen sein?</t>
+  </si>
+  <si>
+    <t>Nur meine Freunde &amp; Freunde von Freunden können alle Informationen von mir einsehen</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Jeder kann auf alle Informationen zugreifen, die ich veröffentliche.</t>
+  </si>
+  <si>
+    <t>Die wichtigsten Daten sind auf privat gestellt, den Rest (z.B) kann aber jeder anschauen</t>
+  </si>
+  <si>
+    <t>Die wichtigsten Daten sind auf privat gestellt, den Rest (z.B) können aber nur meine Freunde ansehen</t>
+  </si>
+  <si>
+    <t>FRAGE5:</t>
+  </si>
+  <si>
+    <t>Was sollte ich bei Zugriffsberechtigungen bedenken?</t>
+  </si>
+  <si>
+    <t>Nichts weiter, wenn jemand fragt, bekommt er diesen.</t>
+  </si>
+  <si>
+    <t>Zugriff sollten immer nur vertrauenswürdige Leute bekommen, und dann nur eingeschränkten, niemals vollen</t>
+  </si>
+  <si>
+    <t>Freunde bekommen vollen Zugriff, unbekannte gar keinen.</t>
+  </si>
+  <si>
+    <t>Jeder der fragt bekommt Zugriff, aber nur eingeschränkten</t>
+  </si>
+  <si>
+    <t>Was sollte beim Hoch- und Runterladen beachtet werden?</t>
+  </si>
+  <si>
+    <t>Filme sind urheberrechtlich geschützt und dürfen nicht runtergeladen werden, Musik ist aber bedenkenlos runterzuladen.</t>
+  </si>
+  <si>
+    <t>Das Hochladen von Filmen, Musik, Ebooks &amp; Hörbüchern ist verboten, das Runterladen aber legal.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sowohl das Hochladen, als auch das illegale Runterladen kostenpflichtiger Inhalte wie Filme, Musik, Ebooks &amp; Hörbüchern ist verboten.  </t>
+  </si>
+  <si>
+    <t>Mich schreibt jemand fremdes im Netz an, worauf sollte ich achten?</t>
+  </si>
+  <si>
+    <t>Viele Dinge werden am Computer mit Passwörtern gesichert, wie wähle ich ein sicheres Passwort?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unbekannte Leute im Internet sind eine Gefahr. Generell sollte ich Unbekannten nie zurückschreiben und auch nicht auf  Internetseiten gehen, die diese mir schicken. </t>
+  </si>
+  <si>
+    <t>Cool, ich bin beliebt! Ich schreibe natürlich zurück.</t>
+  </si>
+  <si>
+    <t>Ich schreibe Fremden nicht zurück, aber die Interseite, die er mir schickt schaue ich mir natürlich an.</t>
+  </si>
+  <si>
+    <t>Wenn jemand fremdes mit mir in einem sozialen Netzwerk befreundet sein möchte, nehme ich die Freundschaft natürlich sofort an.</t>
+  </si>
+  <si>
+    <t>Ich nehme meinen Vornamen mit meinem Geburtsdatum dahinter, das sieht sicher aus.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>abcde oder 12345 sieht leicht aus, ich nehme eins der beiden.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Es gibt nur ein sicheres Passwort, eines was ich mir ausdenke. Ich nehme also Hundeknochen, das hat keinen Bezug zu mir.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Mein sicheres Passwort besteht aus Zahlen, Klein- und Großbuchstaben und Zeichen. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quiz hat keine Dialoge, falls man einen Fehler macht, fängt man von vorne an </t>
+  </si>
+  <si>
+    <t>Alles was ich runterladen kann ist erlaubt, sonst könnt ich es ja nicht runterladen.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -640,6 +784,27 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -725,7 +890,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
@@ -739,6 +904,12 @@
     <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Ausgabe" xfId="5" builtinId="21"/>
@@ -5429,7 +5600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:N48"/>
     </sheetView>
   </sheetViews>
@@ -9869,20 +10040,25 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K51"/>
+  <dimension ref="A1:Y51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -9896,8 +10072,11 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M3" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>61</v>
       </c>
@@ -9932,7 +10111,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>62</v>
       </c>
@@ -9955,7 +10134,7 @@
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>173</v>
       </c>
@@ -9969,8 +10148,20 @@
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M6" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="N6" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -10004,8 +10195,14 @@
       <c r="K7" s="7" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>193</v>
+      </c>
+      <c r="N7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -10019,8 +10216,14 @@
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M8" t="s">
+        <v>194</v>
+      </c>
+      <c r="N8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -10034,8 +10237,14 @@
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M9" t="s">
+        <v>195</v>
+      </c>
+      <c r="N9" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -10049,8 +10258,22 @@
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M10" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="N10" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+      <c r="W10" s="16"/>
+      <c r="X10" s="16"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>172</v>
       </c>
@@ -10064,8 +10287,20 @@
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M11" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -10099,8 +10334,14 @@
       <c r="K12" s="10" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M12" t="s">
+        <v>193</v>
+      </c>
+      <c r="N12" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -10116,8 +10357,20 @@
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M13" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="N13" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="16"/>
+      <c r="T13" s="16"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
@@ -10133,8 +10386,14 @@
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M14" t="s">
+        <v>195</v>
+      </c>
+      <c r="N14" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>3</v>
       </c>
@@ -10150,8 +10409,14 @@
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M15" t="s">
+        <v>196</v>
+      </c>
+      <c r="N15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>174</v>
       </c>
@@ -10165,8 +10430,20 @@
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M16" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="N16" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -10194,8 +10471,14 @@
         <v>150</v>
       </c>
       <c r="K17" s="10"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M17" t="s">
+        <v>193</v>
+      </c>
+      <c r="N17" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
@@ -10209,8 +10492,14 @@
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M18" t="s">
+        <v>194</v>
+      </c>
+      <c r="N18" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>2</v>
       </c>
@@ -10224,8 +10513,23 @@
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" s="16"/>
+      <c r="M19" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="N19" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="16"/>
+      <c r="V19" s="16"/>
+      <c r="W19" s="16"/>
+      <c r="X19" s="16"/>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>3</v>
       </c>
@@ -10239,8 +10543,14 @@
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
       <c r="K20" s="10"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M20" t="s">
+        <v>196</v>
+      </c>
+      <c r="N20" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>175</v>
       </c>
@@ -10254,8 +10564,20 @@
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M21" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="N21" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>1</v>
       </c>
@@ -10271,8 +10593,23 @@
       <c r="K22" s="10" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M22" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="N22" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="16"/>
+      <c r="R22" s="16"/>
+      <c r="S22" s="16"/>
+      <c r="T22" s="16"/>
+      <c r="W22" s="16"/>
+      <c r="X22" s="16"/>
+      <c r="Y22" s="16"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>0</v>
       </c>
@@ -10286,8 +10623,14 @@
       <c r="I23" s="10"/>
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M23" t="s">
+        <v>194</v>
+      </c>
+      <c r="N23" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>2</v>
       </c>
@@ -10301,8 +10644,14 @@
       <c r="I24" s="10"/>
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M24" t="s">
+        <v>195</v>
+      </c>
+      <c r="N24" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>3</v>
       </c>
@@ -10316,8 +10665,14 @@
       <c r="I25" s="10"/>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M25" t="s">
+        <v>196</v>
+      </c>
+      <c r="N25" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>176</v>
       </c>
@@ -10331,8 +10686,20 @@
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M26" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="N26" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>1</v>
       </c>
@@ -10360,8 +10727,14 @@
       </c>
       <c r="J27" s="10"/>
       <c r="K27" s="10"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M27" t="s">
+        <v>193</v>
+      </c>
+      <c r="N27" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>0</v>
       </c>
@@ -10375,8 +10748,14 @@
       <c r="I28" s="10"/>
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M28" t="s">
+        <v>194</v>
+      </c>
+      <c r="N28" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>2</v>
       </c>
@@ -10390,8 +10769,22 @@
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M29" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="N29" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="O29" s="16"/>
+      <c r="P29" s="16"/>
+      <c r="Q29" s="16"/>
+      <c r="R29" s="16"/>
+      <c r="S29" s="16"/>
+      <c r="T29" s="16"/>
+      <c r="W29" s="16"/>
+      <c r="X29" s="16"/>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>3</v>
       </c>
@@ -10405,8 +10798,22 @@
       <c r="I30" s="10"/>
       <c r="J30" s="10"/>
       <c r="K30" s="10"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M30" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="N30" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="O30" s="16"/>
+      <c r="P30" s="16"/>
+      <c r="Q30" s="16"/>
+      <c r="R30" s="16"/>
+      <c r="S30" s="16"/>
+      <c r="T30" s="16"/>
+      <c r="W30" s="16"/>
+      <c r="X30" s="16"/>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>177</v>
       </c>
@@ -10421,7 +10828,7 @@
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>1</v>
       </c>
@@ -10779,5 +11186,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Klickabfolgeplan: Szene 3 überarbeitet
</commit_message>
<xml_diff>
--- a/Klickabfolge Tabelle Szene 1-7.xlsx
+++ b/Klickabfolge Tabelle Szene 1-7.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="-45" windowWidth="28410" windowHeight="12450" activeTab="6"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="28470" windowHeight="12420" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Szene 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1315" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="218">
   <si>
     <t>Interact</t>
   </si>
@@ -211,27 +211,6 @@
     <t>Kein Trigger (Dialog Only)</t>
   </si>
   <si>
-    <t>3.5</t>
-  </si>
-  <si>
-    <t>3.6</t>
-  </si>
-  <si>
-    <t>3.7</t>
-  </si>
-  <si>
-    <t>3.3</t>
-  </si>
-  <si>
-    <t>3.4</t>
-  </si>
-  <si>
-    <t>3.3.4</t>
-  </si>
-  <si>
-    <t>3.3.5</t>
-  </si>
-  <si>
     <t>4.1</t>
   </si>
   <si>
@@ -644,9 +623,6 @@
   </si>
   <si>
     <t>Filme sind urheberrechtlich geschützt und dürfen nicht runtergeladen werden, Musik ist aber bedenkenlos runterzuladen.</t>
-  </si>
-  <si>
-    <t>Das Hochladen von Filmen, Musik, Ebooks &amp; Hörbüchern ist verboten, das Runterladen aber legal.</t>
   </si>
   <si>
     <t xml:space="preserve">Sowohl das Hochladen, als auch das illegale Runterladen kostenpflichtiger Inhalte wie Filme, Musik, Ebooks &amp; Hörbüchern ist verboten.  </t>
@@ -722,6 +698,18 @@
   </si>
   <si>
     <t>Alles was ich runterladen kann ist erlaubt, sonst könnt ich es ja nicht runterladen.</t>
+  </si>
+  <si>
+    <t>Ja Button</t>
+  </si>
+  <si>
+    <t>Nein Button</t>
+  </si>
+  <si>
+    <t>Antivirus Aus</t>
+  </si>
+  <si>
+    <t>Antivirus An</t>
   </si>
 </sst>
 </file>
@@ -1218,8 +1206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA53"/>
   <sheetViews>
-    <sheetView topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:N53"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2625,7 +2613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -3871,18 +3859,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N68"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:N58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -3894,15 +3883,9 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>61</v>
       </c>
@@ -3928,84 +3911,52 @@
         <v>59</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>143</v>
+      </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="I3" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="I3" s="3"/>
       <c r="J3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="8"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="6"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
-      <c r="J4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" s="6"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J4" s="8"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="10" t="s">
+      <c r="B5" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="10" t="s">
@@ -4026,122 +3977,82 @@
       <c r="I5" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N5" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J5" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="10"/>
+      <c r="B6" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
-      <c r="J6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J6" s="10"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="10"/>
+      <c r="B7" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
-      <c r="J7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J7" s="10"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="10"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
-      <c r="J8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="8"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="6"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
-      <c r="J9" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K9" s="6"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="10" t="s">
-        <v>23</v>
-      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="7"/>
       <c r="D10" s="10" t="s">
         <v>23</v>
       </c>
@@ -4160,108 +4071,72 @@
       <c r="I10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K10" s="7"/>
-      <c r="L10" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M10" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N10" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J10" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="10"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="7"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
-      <c r="J11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K11" s="7"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="10"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="7"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
-      <c r="J12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K12" s="7"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="10"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="7"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
-      <c r="J13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K13" s="7"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="8"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="6"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
-      <c r="J14" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K14" s="6"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="10" t="s">
-        <v>23</v>
-      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="7"/>
       <c r="D15" s="10" t="s">
         <v>23</v>
       </c>
@@ -4280,116 +4155,76 @@
       <c r="I15" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K15" s="7"/>
-      <c r="L15" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M15" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N15" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J15" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="10"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
-      <c r="J16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K16" s="7"/>
-      <c r="L16" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="10"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="7"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
-      <c r="J17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K17" s="7"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J17" s="10"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="10" t="s">
+      <c r="B18" s="2"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
-      <c r="J18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K18" s="7"/>
-      <c r="L18" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J18" s="10"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="8"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="6"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
-      <c r="J19" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="K19" s="6"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J19" s="8"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="10" t="s">
-        <v>23</v>
-      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="7"/>
       <c r="D20" s="10" t="s">
         <v>23</v>
       </c>
@@ -4405,92 +4240,62 @@
       <c r="H20" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I20" s="10"/>
-      <c r="J20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K20" s="7"/>
-      <c r="L20" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M20" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N20" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I20" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="10"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>143</v>
+      </c>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
-      <c r="J21" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K21" s="7"/>
-      <c r="L21" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J21" s="10"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="10"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="7"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
-      <c r="J22" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K22" s="7"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J22" s="10"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="10" t="s">
+      <c r="B23" s="2"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
-      <c r="J23" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K23" s="7"/>
-      <c r="L23" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J23" s="10"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>46</v>
+        <v>216</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -4500,22 +4305,16 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
-      <c r="J24" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="10" t="s">
-        <v>23</v>
-      </c>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="7"/>
       <c r="D25" s="10" t="s">
-        <v>23</v>
+        <v>143</v>
       </c>
       <c r="E25" s="10" t="s">
         <v>23</v>
@@ -4530,1065 +4329,367 @@
         <v>23</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J25" s="2"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M25" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N25" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="10" t="s">
-        <v>23</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="J25" s="10"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="7"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="J28" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K28" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="L28" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="M28" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="N28" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J29" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N29" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K30" s="6"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J26" s="10"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F31" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H31" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I31" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K31" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="L31" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M31" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N31" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" s="10"/>
+        <v>2</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="7"/>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
       <c r="I32" s="10"/>
-      <c r="J32" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K32" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
-      <c r="N32" s="10"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J32" s="10"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" s="10"/>
+        <v>3</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="7"/>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
       <c r="I33" s="10"/>
-      <c r="J33" s="2" t="s">
+      <c r="J33" s="10"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I35" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J35" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K33" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="L33" s="10"/>
-      <c r="M33" s="10"/>
-      <c r="N33" s="10"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K34" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="L34" s="10"/>
-      <c r="M34" s="10"/>
-      <c r="N34" s="10"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K35" s="6"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F36" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I36" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K36" s="7"/>
-      <c r="L36" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M36" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N36" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37" s="7"/>
-      <c r="C37" s="10"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="7"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
       <c r="H37" s="10"/>
       <c r="I37" s="10"/>
-      <c r="J37" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K37" s="7"/>
-      <c r="L37" s="10"/>
-      <c r="M37" s="10"/>
-      <c r="N37" s="10"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J37" s="10"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="10"/>
+        <v>3</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="7"/>
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
+      <c r="F38" s="10" t="s">
+        <v>60</v>
+      </c>
       <c r="G38" s="10"/>
       <c r="H38" s="10"/>
       <c r="I38" s="10"/>
-      <c r="J38" s="2" t="s">
+      <c r="J38" s="10"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I40" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J40" s="10"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="J41" s="10"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K38" s="7"/>
-      <c r="L38" s="10"/>
-      <c r="M38" s="10"/>
-      <c r="N38" s="10"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B39" s="7"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K39" s="7"/>
-      <c r="L39" s="10"/>
-      <c r="M39" s="10"/>
-      <c r="N39" s="10"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" s="6"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K40" s="6"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
-      <c r="N40" s="8"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B41" s="7"/>
-      <c r="C41" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E41" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F41" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G41" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H41" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I41" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K41" s="7"/>
-      <c r="L41" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M41" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N41" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B42" s="7"/>
-      <c r="C42" s="10" t="s">
-        <v>23</v>
-      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="7"/>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
       <c r="H42" s="10"/>
       <c r="I42" s="10"/>
-      <c r="J42" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K42" s="7"/>
-      <c r="L42" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M42" s="10"/>
-      <c r="N42" s="10"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J42" s="10"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B43" s="7"/>
-      <c r="C43" s="10"/>
+        <v>3</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" s="7"/>
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
       <c r="H43" s="10"/>
-      <c r="I43" s="10"/>
-      <c r="J43" s="2" t="s">
+      <c r="I43" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="J43" s="10"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" s="2"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I45" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J45" s="10"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="2"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="I46" s="10"/>
+      <c r="J46" s="10"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K43" s="7"/>
-      <c r="L43" s="10"/>
-      <c r="M43" s="10"/>
-      <c r="N43" s="10"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B44" s="7"/>
-      <c r="C44" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
-      <c r="H44" s="10"/>
-      <c r="I44" s="10"/>
-      <c r="J44" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K44" s="7"/>
-      <c r="L44" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="M44" s="10"/>
-      <c r="N44" s="10"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B45" s="6"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
-      <c r="J45" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="K45" s="6"/>
-      <c r="L45" s="8"/>
-      <c r="M45" s="8"/>
-      <c r="N45" s="8"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B46" s="7"/>
-      <c r="C46" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D46" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F46" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G46" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H46" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I46" s="10"/>
-      <c r="J46" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K46" s="7"/>
-      <c r="L46" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M46" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N46" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="7"/>
-      <c r="C47" s="10" t="s">
-        <v>23</v>
-      </c>
+      <c r="B47" s="2"/>
+      <c r="C47" s="7"/>
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
       <c r="G47" s="10"/>
       <c r="H47" s="10"/>
       <c r="I47" s="10"/>
-      <c r="J47" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K47" s="7"/>
-      <c r="L47" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M47" s="10"/>
-      <c r="N47" s="10"/>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J47" s="10"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="10"/>
+        <v>3</v>
+      </c>
+      <c r="B48" s="2"/>
+      <c r="C48" s="7"/>
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
       <c r="G48" s="10"/>
-      <c r="H48" s="10"/>
+      <c r="H48" s="10" t="s">
+        <v>143</v>
+      </c>
       <c r="I48" s="10"/>
-      <c r="J48" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K48" s="7"/>
-      <c r="L48" s="10"/>
-      <c r="M48" s="10"/>
-      <c r="N48" s="10"/>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B49" s="7"/>
-      <c r="C49" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="10"/>
-      <c r="H49" s="10"/>
-      <c r="I49" s="10"/>
-      <c r="J49" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K49" s="7"/>
-      <c r="L49" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="M49" s="10"/>
-      <c r="N49" s="10"/>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
-      <c r="I50" s="4"/>
-      <c r="J50" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="K50" s="4"/>
-      <c r="L50" s="4"/>
-      <c r="M50" s="4"/>
-      <c r="N50" s="4"/>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" s="2"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D51" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E51" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F51" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G51" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H51" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I51" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J51" s="2"/>
-      <c r="K51" s="7"/>
-      <c r="L51" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M51" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N51" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="2"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="10"/>
-      <c r="G52" s="10"/>
-      <c r="H52" s="10"/>
-      <c r="I52" s="10"/>
-      <c r="J52" s="2"/>
-      <c r="K52" s="7"/>
-      <c r="L52" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M52" s="10"/>
-      <c r="N52" s="10"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G54" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H54" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="I54" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="J54" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K54" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="L54" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="M54" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="N54" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J55" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="K55" s="3"/>
-      <c r="L55" s="3"/>
-      <c r="M55" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N55" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B56" s="6"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
-      <c r="F56" s="8"/>
-      <c r="G56" s="8"/>
-      <c r="H56" s="8"/>
-      <c r="I56" s="8"/>
-      <c r="J56" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K56" s="6"/>
-      <c r="L56" s="8"/>
-      <c r="M56" s="8"/>
-      <c r="N56" s="8"/>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C57" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D57" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E57" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F57" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G57" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H57" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I57" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J57" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K57" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="L57" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M57" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N57" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="10"/>
-      <c r="G58" s="10"/>
-      <c r="H58" s="10"/>
-      <c r="I58" s="10"/>
-      <c r="J58" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K58" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="L58" s="10"/>
-      <c r="M58" s="10"/>
-      <c r="N58" s="10"/>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
-      <c r="B59" s="6"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="8"/>
-      <c r="E59" s="8"/>
-      <c r="F59" s="8"/>
-      <c r="G59" s="8"/>
-      <c r="H59" s="8"/>
-      <c r="I59" s="8"/>
-      <c r="J59" s="8"/>
-      <c r="K59" s="8"/>
-      <c r="L59" s="8"/>
-      <c r="M59" s="8"/>
-      <c r="N59" s="9"/>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" s="2"/>
-      <c r="B60" s="7"/>
-      <c r="C60" s="7"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="7"/>
-      <c r="G60" s="7"/>
-      <c r="H60" s="7"/>
-      <c r="I60" s="7"/>
-      <c r="J60" s="7"/>
-      <c r="K60" s="7"/>
-      <c r="L60" s="7"/>
-      <c r="M60" s="7"/>
-      <c r="N60" s="2"/>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A61" s="2"/>
-      <c r="B61" s="7"/>
-      <c r="C61" s="7"/>
-      <c r="D61" s="7"/>
-      <c r="E61" s="7"/>
-      <c r="F61" s="7"/>
-      <c r="G61" s="7"/>
-      <c r="H61" s="7"/>
-      <c r="I61" s="7"/>
-      <c r="J61" s="7"/>
-      <c r="K61" s="7"/>
-      <c r="L61" s="7"/>
-      <c r="M61" s="7"/>
-      <c r="N61" s="2"/>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A62" s="2"/>
-      <c r="B62" s="7"/>
-      <c r="C62" s="7"/>
-      <c r="D62" s="7"/>
-      <c r="E62" s="7"/>
-      <c r="F62" s="7"/>
-      <c r="G62" s="7"/>
-      <c r="H62" s="7"/>
-      <c r="I62" s="7"/>
-      <c r="J62" s="7"/>
-      <c r="K62" s="7"/>
-      <c r="L62" s="7"/>
-      <c r="M62" s="7"/>
-      <c r="N62" s="2"/>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A63" s="2"/>
-      <c r="B63" s="7"/>
-      <c r="C63" s="7"/>
-      <c r="D63" s="7"/>
-      <c r="E63" s="7"/>
-      <c r="F63" s="7"/>
-      <c r="G63" s="7"/>
-      <c r="H63" s="7"/>
-      <c r="I63" s="7"/>
-      <c r="J63" s="7"/>
-      <c r="K63" s="7"/>
-      <c r="L63" s="7"/>
-      <c r="M63" s="7"/>
-      <c r="N63" s="2"/>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
-      <c r="B64" s="6"/>
-      <c r="C64" s="6"/>
-      <c r="D64" s="6"/>
-      <c r="E64" s="6"/>
-      <c r="F64" s="6"/>
-      <c r="G64" s="6"/>
-      <c r="H64" s="6"/>
-      <c r="I64" s="6"/>
-      <c r="J64" s="6"/>
-      <c r="K64" s="6"/>
-      <c r="L64" s="6"/>
-      <c r="M64" s="6"/>
-      <c r="N64" s="4"/>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A65" s="2"/>
-      <c r="B65" s="7"/>
-      <c r="C65" s="7"/>
-      <c r="D65" s="7"/>
-      <c r="E65" s="7"/>
-      <c r="F65" s="7"/>
-      <c r="G65" s="7"/>
-      <c r="H65" s="7"/>
-      <c r="I65" s="7"/>
-      <c r="J65" s="7"/>
-      <c r="K65" s="7"/>
-      <c r="L65" s="7"/>
-      <c r="M65" s="7"/>
-      <c r="N65" s="2"/>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A66" s="2"/>
-      <c r="B66" s="7"/>
-      <c r="C66" s="7"/>
-      <c r="D66" s="7"/>
-      <c r="E66" s="7"/>
-      <c r="F66" s="7"/>
-      <c r="G66" s="7"/>
-      <c r="H66" s="7"/>
-      <c r="I66" s="7"/>
-      <c r="J66" s="7"/>
-      <c r="K66" s="7"/>
-      <c r="L66" s="7"/>
-      <c r="M66" s="7"/>
-      <c r="N66" s="2"/>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A67" s="2"/>
-      <c r="B67" s="7"/>
-      <c r="C67" s="7"/>
-      <c r="D67" s="7"/>
-      <c r="E67" s="7"/>
-      <c r="F67" s="7"/>
-      <c r="G67" s="7"/>
-      <c r="H67" s="7"/>
-      <c r="I67" s="7"/>
-      <c r="J67" s="7"/>
-      <c r="K67" s="7"/>
-      <c r="L67" s="7"/>
-      <c r="M67" s="7"/>
-      <c r="N67" s="2"/>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A68" s="2"/>
-      <c r="B68" s="7"/>
-      <c r="C68" s="7"/>
-      <c r="D68" s="7"/>
-      <c r="E68" s="7"/>
-      <c r="F68" s="7"/>
-      <c r="G68" s="7"/>
-      <c r="H68" s="7"/>
-      <c r="I68" s="7"/>
-      <c r="J68" s="7"/>
-      <c r="K68" s="7"/>
-      <c r="L68" s="7"/>
-      <c r="M68" s="7"/>
-      <c r="N68" s="2"/>
+      <c r="J48" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -5632,37 +4733,37 @@
         <v>61</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="I2" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>80</v>
       </c>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
@@ -5693,7 +4794,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="8"/>
@@ -5791,7 +4892,7 @@
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
@@ -5805,7 +4906,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="8"/>
@@ -5904,7 +5005,7 @@
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
@@ -5917,7 +5018,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="8"/>
@@ -6021,7 +5122,7 @@
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
@@ -6033,7 +5134,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="8"/>
@@ -6125,7 +5226,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="8"/>
@@ -6223,7 +5324,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="8"/>
@@ -6319,7 +5420,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="8"/>
@@ -6415,7 +5516,7 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="8"/>
@@ -6513,7 +5614,7 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B44" s="6"/>
       <c r="C44" s="8"/>
@@ -6636,7 +5737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
@@ -6644,20 +5745,20 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -6690,64 +5791,64 @@
         <v>61</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="H5" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="L5" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="M5" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q5" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="R5" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="S5" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="L5" s="5" t="s">
+      <c r="T5" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="U5" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="P5" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q5" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="R5" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="S5" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="T5" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="U5" s="5" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -6771,7 +5872,7 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
@@ -6785,7 +5886,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="8"/>
@@ -6930,7 +6031,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="8"/>
@@ -7061,7 +6162,7 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="8"/>
@@ -7204,7 +6305,7 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="8"/>
@@ -7361,7 +6462,7 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="9"/>
@@ -7446,7 +6547,7 @@
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="10"/>
@@ -7471,7 +6572,7 @@
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="10"/>
@@ -7496,7 +6597,7 @@
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="8"/>
@@ -7617,7 +6718,7 @@
       </c>
       <c r="I36" s="10"/>
       <c r="J36" s="2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="K36" s="7"/>
       <c r="L36" s="10"/>
@@ -7633,7 +6734,7 @@
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="8"/>
@@ -7756,7 +6857,7 @@
         <v>23</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="K41" s="7"/>
       <c r="L41" s="10"/>
@@ -7772,7 +6873,7 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B42" s="6"/>
       <c r="C42" s="8"/>
@@ -7931,7 +7032,7 @@
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B47" s="6"/>
       <c r="C47" s="8"/>
@@ -8080,7 +7181,7 @@
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B52" s="6"/>
       <c r="C52" s="8"/>
@@ -8215,7 +7316,7 @@
         <v>23</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="K56" s="7"/>
       <c r="L56" s="10"/>
@@ -8223,7 +7324,7 @@
       <c r="N56" s="10"/>
       <c r="O56" s="2"/>
       <c r="P56" s="7" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="Q56" s="10"/>
       <c r="R56" s="10"/>
@@ -8233,7 +7334,7 @@
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B57" s="6"/>
       <c r="C57" s="8"/>
@@ -8364,7 +7465,7 @@
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B62" s="6"/>
       <c r="C62" s="8"/>
@@ -8495,7 +7596,7 @@
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B67" s="6"/>
       <c r="C67" s="8"/>
@@ -8626,7 +7727,7 @@
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B72" s="6"/>
       <c r="C72" s="8"/>
@@ -8772,12 +7873,12 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -8803,37 +7904,37 @@
         <v>61</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>133</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>140</v>
       </c>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
@@ -8843,12 +7944,12 @@
         <v>62</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="12" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
@@ -8857,14 +7958,14 @@
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="8"/>
@@ -8885,37 +7986,37 @@
         <v>1</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
@@ -8926,7 +8027,7 @@
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -8964,7 +8065,7 @@
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -8980,7 +8081,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="8"/>
@@ -9001,19 +8102,19 @@
         <v>1</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
@@ -9033,7 +8134,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
@@ -9049,19 +8150,19 @@
         <v>2</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
@@ -9081,7 +8182,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
@@ -9094,7 +8195,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="8"/>
@@ -9120,22 +8221,22 @@
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="L17" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
@@ -9150,7 +8251,7 @@
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
@@ -9170,19 +8271,19 @@
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
@@ -9198,7 +8299,7 @@
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
@@ -9210,7 +8311,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="8"/>
@@ -9231,34 +8332,34 @@
         <v>1</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="L22" s="10"/>
       <c r="M22" s="10"/>
@@ -9271,7 +8372,7 @@
       <c r="B23" s="7"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
@@ -9290,31 +8391,31 @@
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="L24" s="10"/>
       <c r="M24" s="10"/>
@@ -9327,7 +8428,7 @@
       <c r="B25" s="7"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
@@ -9342,7 +8443,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="8"/>
@@ -9373,7 +8474,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="7"/>
       <c r="L27" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="M27" s="10"/>
       <c r="N27" s="10"/>
@@ -9434,7 +8535,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="8"/>
@@ -9455,37 +8556,37 @@
         <v>1</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="K32" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="L32" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="M32" s="7"/>
       <c r="N32" s="7"/>
@@ -9513,34 +8614,34 @@
         <v>2</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="I34" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="K34" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="L34" s="10"/>
       <c r="M34" s="10"/>
@@ -9566,7 +8667,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="8"/>
@@ -9595,13 +8696,13 @@
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
       <c r="J37" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="K37" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="L37" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="M37" s="7"/>
       <c r="N37" s="7"/>
@@ -9619,10 +8720,10 @@
       <c r="H38" s="10"/>
       <c r="I38" s="10"/>
       <c r="J38" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="K38" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="L38" s="10"/>
       <c r="M38" s="10"/>
@@ -9659,10 +8760,10 @@
       <c r="H40" s="10"/>
       <c r="I40" s="10"/>
       <c r="J40" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="K40" s="7" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="L40" s="10"/>
       <c r="M40" s="10"/>
@@ -9670,7 +8771,7 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="8"/>
@@ -9699,13 +8800,13 @@
       <c r="H42" s="7"/>
       <c r="I42" s="7"/>
       <c r="J42" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="K42" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="L42" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="M42" s="7"/>
       <c r="N42" s="7"/>
@@ -9723,10 +8824,10 @@
       <c r="H43" s="10"/>
       <c r="I43" s="10"/>
       <c r="J43" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="K43" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="L43" s="10"/>
       <c r="M43" s="10"/>
@@ -9763,10 +8864,10 @@
       <c r="H45" s="10"/>
       <c r="I45" s="10"/>
       <c r="J45" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K45" s="7" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="L45" s="10"/>
       <c r="M45" s="10"/>
@@ -9774,7 +8875,7 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B46" s="6"/>
       <c r="C46" s="8"/>
@@ -9803,13 +8904,13 @@
       <c r="H47" s="7"/>
       <c r="I47" s="7"/>
       <c r="J47" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="K47" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="L47" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="M47" s="7"/>
       <c r="N47" s="7"/>
@@ -9827,10 +8928,10 @@
       <c r="H48" s="10"/>
       <c r="I48" s="10"/>
       <c r="J48" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="K48" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="L48" s="10"/>
       <c r="M48" s="10"/>
@@ -9867,10 +8968,10 @@
       <c r="H50" s="10"/>
       <c r="I50" s="10"/>
       <c r="J50" s="2" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="K50" s="7" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="L50" s="10"/>
       <c r="M50" s="10"/>
@@ -9878,7 +8979,7 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B51" s="6"/>
       <c r="C51" s="8"/>
@@ -9896,7 +8997,7 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="11"/>
@@ -9905,7 +9006,7 @@
       <c r="F52" s="11"/>
       <c r="G52" s="11"/>
       <c r="H52" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="I52" s="11"/>
       <c r="J52" s="2"/>
@@ -9916,47 +9017,47 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="I53" s="10" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="K53" s="7" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="L53" s="10" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="M53" s="10"/>
       <c r="N53" s="10"/>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B54" s="6"/>
       <c r="C54" s="8"/>
@@ -9974,7 +9075,7 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="11"/>
@@ -9984,7 +9085,7 @@
       <c r="G55" s="11"/>
       <c r="H55" s="11"/>
       <c r="I55" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
@@ -9994,40 +9095,40 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="I56" s="7" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="K56" s="7" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="L56" s="10" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="M56" s="10"/>
       <c r="N56" s="10"/>
@@ -10042,7 +9143,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
@@ -10050,12 +9151,12 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
@@ -10073,7 +9174,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
@@ -10081,34 +9182,34 @@
         <v>61</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -10116,27 +9217,27 @@
         <v>62</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="8"/>
@@ -10149,10 +9250,10 @@
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="M6" s="13" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="N6" s="15" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -10166,40 +9267,40 @@
         <v>1</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="M7" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="N7" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
@@ -10217,10 +9318,10 @@
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
       <c r="M8" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="N8" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
@@ -10238,10 +9339,10 @@
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
       <c r="M9" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="N9" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
@@ -10259,10 +9360,10 @@
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
       <c r="M10" s="16" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="N10" s="16" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="O10" s="16"/>
       <c r="P10" s="16"/>
@@ -10275,7 +9376,7 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="8"/>
@@ -10288,10 +9389,10 @@
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="M11" s="1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -10305,40 +9406,40 @@
         <v>1</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="M12" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="N12" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
@@ -10351,17 +9452,17 @@
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
       <c r="M13" s="16" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="N13" s="16" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="O13" s="16"/>
       <c r="P13" s="16"/>
@@ -10380,17 +9481,17 @@
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
       <c r="M14" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="N14" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
@@ -10403,22 +9504,22 @@
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
       <c r="M15" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="N15" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="8"/>
@@ -10431,10 +9532,10 @@
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
       <c r="M16" s="1" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="N16" s="14" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="O16" s="14"/>
       <c r="P16" s="14"/>
@@ -10448,34 +9549,34 @@
         <v>1</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
       <c r="I17" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="K17" s="10"/>
       <c r="M17" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="N17" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
@@ -10493,10 +9594,10 @@
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
       <c r="M18" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="N18" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
@@ -10515,10 +9616,10 @@
       <c r="K19" s="10"/>
       <c r="L19" s="16"/>
       <c r="M19" s="16" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="N19" s="16" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="O19" s="16"/>
       <c r="P19" s="16"/>
@@ -10544,15 +9645,15 @@
       <c r="J20" s="10"/>
       <c r="K20" s="10"/>
       <c r="M20" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="N20" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="8"/>
@@ -10565,10 +9666,10 @@
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
       <c r="M21" s="1" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="N21" s="15" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
@@ -10591,13 +9692,13 @@
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
       <c r="K22" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="M22" s="16" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="N22" s="16" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="O22" s="16"/>
       <c r="P22" s="16"/>
@@ -10624,10 +9725,10 @@
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
       <c r="M23" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="N23" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
@@ -10645,10 +9746,10 @@
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
       <c r="M24" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="N24" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
@@ -10666,15 +9767,15 @@
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
       <c r="M25" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="N25" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="8"/>
@@ -10687,10 +9788,10 @@
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
       <c r="M26" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="N26" s="14" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
@@ -10704,34 +9805,34 @@
         <v>1</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="H27" s="10"/>
       <c r="I27" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="J27" s="10"/>
       <c r="K27" s="10"/>
       <c r="M27" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="N27" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
@@ -10749,10 +9850,10 @@
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
       <c r="M28" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="N28" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
@@ -10770,10 +9871,10 @@
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
       <c r="M29" s="16" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="N29" s="16" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="O29" s="16"/>
       <c r="P29" s="16"/>
@@ -10799,10 +9900,10 @@
       <c r="J30" s="10"/>
       <c r="K30" s="10"/>
       <c r="M30" s="16" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="N30" s="16" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="O30" s="16"/>
       <c r="P30" s="16"/>
@@ -10815,7 +9916,7 @@
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="8"/>
@@ -10837,13 +9938,13 @@
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
       <c r="F32" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
       <c r="J32" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="K32" s="2"/>
     </row>
@@ -10856,13 +9957,13 @@
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
       <c r="F33" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
       <c r="I33" s="10"/>
       <c r="J33" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="K33" s="2"/>
     </row>
@@ -10890,19 +9991,19 @@
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
       <c r="F35" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="G35" s="10"/>
       <c r="H35" s="10"/>
       <c r="I35" s="10"/>
       <c r="J35" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="K35" s="2"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="8"/>
@@ -10920,31 +10021,31 @@
         <v>1</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="J37" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="K37" s="7"/>
     </row>
@@ -10995,7 +10096,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="8"/>
@@ -11022,7 +10123,7 @@
       <c r="I42" s="7"/>
       <c r="J42" s="7"/>
       <c r="K42" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -11072,7 +10173,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="B46" s="6"/>
       <c r="C46" s="8"/>
@@ -11090,32 +10191,32 @@
         <v>1</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F47" s="11" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="H47" s="11"/>
       <c r="I47" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="J47" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="K47" s="11" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -11126,7 +10227,7 @@
       <c r="C48" s="11"/>
       <c r="D48" s="11"/>
       <c r="E48" s="11" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F48" s="11"/>
       <c r="G48" s="11"/>
@@ -11158,7 +10259,7 @@
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
@@ -11169,7 +10270,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -11181,7 +10282,7 @@
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>